<commit_message>
Criei um novo dataframe com os tweets limpo de pontuacao e com os espacos ajustados
</commit_message>
<xml_diff>
--- a/Golf.xlsx
+++ b/Golf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisf\OneDrive - Insper - Institudo de Ensino e Pesquisa\Documentos\INSPER\SEGUNDO SEMESTRE\Ciência dos Dados\Projeto_2\Projeto2_CD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391E7157-5427-48EC-8345-22D2A5A86967}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74FFD0F1-CD94-4B0C-BAF8-E2162A1DDE2F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="753">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="754">
   <si>
     <t>Treinamento</t>
   </si>
@@ -2778,6 +2778,9 @@
   </si>
   <si>
     <t>amei dirigir o golf, quero um agora</t>
+  </si>
+  <si>
+    <t>Relevancia</t>
   </si>
 </sst>
 </file>
@@ -2836,11 +2839,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3181,18 +3185,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A203" zoomScale="83" zoomScaleNormal="83" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" zoomScaleSheetLayoutView="50" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="168.08984375" customWidth="1"/>
+    <col min="2" max="2" width="10.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>753</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Arrumando 2 tweets errados
</commit_message>
<xml_diff>
--- a/Golf.xlsx
+++ b/Golf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisf\OneDrive - Insper - Institudo de Ensino e Pesquisa\Documentos\INSPER\SEGUNDO SEMESTRE\Ciência dos Dados\Projeto_2\Projeto2_CD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74FFD0F1-CD94-4B0C-BAF8-E2162A1DDE2F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1201EC-9A30-487F-9576-27361F5CD74C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3186,7 +3186,7 @@
   <dimension ref="A1:B501"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3296,7 +3296,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
@@ -3368,7 +3368,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Arrumado o teorema e feito o laplace
</commit_message>
<xml_diff>
--- a/Golf.xlsx
+++ b/Golf.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisf\OneDrive - Insper - Institudo de Ensino e Pesquisa\Documentos\INSPER\SEGUNDO SEMESTRE\Ciência dos Dados\Projeto_2\Projeto2_CD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1201EC-9A30-487F-9576-27361F5CD74C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{381342C0-50B1-4775-9AAB-F40B7432BD81}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="754">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="754">
   <si>
     <t>Treinamento</t>
   </si>
@@ -2285,9 +2285,6 @@
     <t>amas é agora mesmo que ela não sai do campo de golf https://t.co/a0oxvveefr</t>
   </si>
   <si>
-    <t>@lin___d a gente vai e sair dando grau no golf</t>
-  </si>
-  <si>
     <t>fim da produção do vw golf 1.0 e 1.4 no brasil - https://t.co/584bdxq5r7</t>
   </si>
   <si>
@@ -2781,6 +2778,9 @@
   </si>
   <si>
     <t>Relevancia</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> a gente vai e sair dando grau no golf</t>
   </si>
 </sst>
 </file>
@@ -3185,8 +3185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B501"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView zoomScale="83" zoomScaleNormal="83" zoomScaleSheetLayoutView="50" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3200,7 +3200,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -7213,19 +7213,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B252"/>
   <sheetViews>
-    <sheetView topLeftCell="A260" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="A288" sqref="A288"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="A139" sqref="A139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="168.08984375" customWidth="1"/>
+    <col min="2" max="2" width="11.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>501</v>
       </c>
+      <c r="B1" s="2" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -8149,7 +8153,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>617</v>
+        <v>753</v>
       </c>
       <c r="B117">
         <v>1</v>
@@ -8157,7 +8161,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B118">
         <v>1</v>
@@ -8165,7 +8169,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B119">
         <v>0</v>
@@ -8173,7 +8177,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B120">
         <v>1</v>
@@ -8181,7 +8185,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B121">
         <v>2</v>
@@ -8189,7 +8193,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B122">
         <v>0</v>
@@ -8197,7 +8201,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B123">
         <v>0</v>
@@ -8205,7 +8209,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B124">
         <v>0</v>
@@ -8213,7 +8217,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B125">
         <v>1</v>
@@ -8221,7 +8225,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B126">
         <v>2</v>
@@ -8229,7 +8233,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B127">
         <v>0</v>
@@ -8237,7 +8241,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B128">
         <v>0</v>
@@ -8245,7 +8249,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B129">
         <v>1</v>
@@ -8253,7 +8257,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B130">
         <v>0</v>
@@ -8261,7 +8265,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B131">
         <v>0</v>
@@ -8269,7 +8273,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B132">
         <v>0</v>
@@ -8277,7 +8281,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B133">
         <v>0</v>
@@ -8285,7 +8289,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B134">
         <v>0</v>
@@ -8293,7 +8297,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B135">
         <v>0</v>
@@ -8301,7 +8305,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B136">
         <v>0</v>
@@ -8309,7 +8313,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B137">
         <v>0</v>
@@ -8317,7 +8321,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B138">
         <v>1</v>
@@ -8325,7 +8329,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B139">
         <v>0</v>
@@ -8333,7 +8337,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B140">
         <v>2</v>
@@ -8341,7 +8345,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B141">
         <v>1</v>
@@ -8349,7 +8353,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B142">
         <v>0</v>
@@ -8357,7 +8361,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B143">
         <v>0</v>
@@ -8365,7 +8369,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B144">
         <v>0</v>
@@ -8373,7 +8377,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B145">
         <v>0</v>
@@ -8381,7 +8385,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B146">
         <v>0</v>
@@ -8389,7 +8393,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B147">
         <v>0</v>
@@ -8397,7 +8401,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B148">
         <v>0</v>
@@ -8405,7 +8409,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B149">
         <v>2</v>
@@ -8413,7 +8417,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B150">
         <v>0</v>
@@ -8421,7 +8425,7 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B151">
         <v>1</v>
@@ -8429,7 +8433,7 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B152">
         <v>1</v>
@@ -8437,7 +8441,7 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B153">
         <v>0</v>
@@ -8445,7 +8449,7 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B154">
         <v>0</v>
@@ -8453,7 +8457,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B155">
         <v>0</v>
@@ -8461,7 +8465,7 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B156">
         <v>2</v>
@@ -8469,7 +8473,7 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B157">
         <v>0</v>
@@ -8477,7 +8481,7 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B158">
         <v>2</v>
@@ -8485,7 +8489,7 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B159">
         <v>1</v>
@@ -8493,7 +8497,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B160">
         <v>0</v>
@@ -8501,7 +8505,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B161">
         <v>1</v>
@@ -8509,7 +8513,7 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B162">
         <v>0</v>
@@ -8517,7 +8521,7 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B163">
         <v>0</v>
@@ -8525,7 +8529,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B164">
         <v>2</v>
@@ -8533,7 +8537,7 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B165">
         <v>2</v>
@@ -8541,7 +8545,7 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B166">
         <v>1</v>
@@ -8549,7 +8553,7 @@
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B167">
         <v>1</v>
@@ -8557,7 +8561,7 @@
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B168">
         <v>0</v>
@@ -8565,7 +8569,7 @@
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B169">
         <v>0</v>
@@ -8573,7 +8577,7 @@
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B170">
         <v>0</v>
@@ -8581,7 +8585,7 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B171">
         <v>0</v>
@@ -8589,7 +8593,7 @@
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B172">
         <v>1</v>
@@ -8597,7 +8601,7 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B173">
         <v>1</v>
@@ -8605,7 +8609,7 @@
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B174">
         <v>0</v>
@@ -8613,7 +8617,7 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B175">
         <v>0</v>
@@ -8621,7 +8625,7 @@
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B176">
         <v>0</v>
@@ -8629,7 +8633,7 @@
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B177">
         <v>0</v>
@@ -8637,7 +8641,7 @@
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B178">
         <v>2</v>
@@ -8645,7 +8649,7 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B179">
         <v>0</v>
@@ -8653,7 +8657,7 @@
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B180">
         <v>0</v>
@@ -8661,7 +8665,7 @@
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B181">
         <v>1</v>
@@ -8669,7 +8673,7 @@
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B182">
         <v>2</v>
@@ -8677,7 +8681,7 @@
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B183">
         <v>0</v>
@@ -8685,7 +8689,7 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B184">
         <v>0</v>
@@ -8693,7 +8697,7 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B185">
         <v>0</v>
@@ -8701,7 +8705,7 @@
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B186">
         <v>1</v>
@@ -8709,7 +8713,7 @@
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B187">
         <v>1</v>
@@ -8717,7 +8721,7 @@
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B188">
         <v>0</v>
@@ -8725,7 +8729,7 @@
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B189">
         <v>0</v>
@@ -8733,7 +8737,7 @@
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B190">
         <v>0</v>
@@ -8741,7 +8745,7 @@
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B191">
         <v>0</v>
@@ -8749,7 +8753,7 @@
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="B192">
         <v>2</v>
@@ -8757,7 +8761,7 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="B193">
         <v>0</v>
@@ -8765,7 +8769,7 @@
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="B194">
         <v>0</v>
@@ -8773,7 +8777,7 @@
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B195">
         <v>0</v>
@@ -8781,7 +8785,7 @@
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="B196">
         <v>1</v>
@@ -8789,7 +8793,7 @@
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="B197">
         <v>0</v>
@@ -8797,7 +8801,7 @@
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="B198">
         <v>1</v>
@@ -8805,7 +8809,7 @@
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B199">
         <v>0</v>
@@ -8813,7 +8817,7 @@
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B200">
         <v>0</v>
@@ -8821,7 +8825,7 @@
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B201">
         <v>0</v>
@@ -8829,7 +8833,7 @@
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B202">
         <v>0</v>
@@ -8837,7 +8841,7 @@
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B203">
         <v>0</v>
@@ -8845,7 +8849,7 @@
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="B204">
         <v>0</v>
@@ -8853,7 +8857,7 @@
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="B205">
         <v>0</v>
@@ -8861,7 +8865,7 @@
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B206">
         <v>2</v>
@@ -8869,7 +8873,7 @@
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B207">
         <v>0</v>
@@ -8877,7 +8881,7 @@
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B208">
         <v>2</v>
@@ -8885,7 +8889,7 @@
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="B209">
         <v>2</v>
@@ -8893,7 +8897,7 @@
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="B210">
         <v>0</v>
@@ -8901,7 +8905,7 @@
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="B211">
         <v>2</v>
@@ -8909,7 +8913,7 @@
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="B212">
         <v>2</v>
@@ -8917,7 +8921,7 @@
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="B213">
         <v>0</v>
@@ -8925,7 +8929,7 @@
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="B214">
         <v>0</v>
@@ -8933,7 +8937,7 @@
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="B215">
         <v>0</v>
@@ -8941,7 +8945,7 @@
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="B216">
         <v>0</v>
@@ -8949,7 +8953,7 @@
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="B217">
         <v>1</v>
@@ -8957,7 +8961,7 @@
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="B218">
         <v>0</v>
@@ -8965,7 +8969,7 @@
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B219">
         <v>0</v>
@@ -8973,7 +8977,7 @@
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B220">
         <v>1</v>
@@ -8981,7 +8985,7 @@
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="B221">
         <v>0</v>
@@ -8989,7 +8993,7 @@
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="B222">
         <v>1</v>
@@ -8997,7 +9001,7 @@
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B223">
         <v>1</v>
@@ -9005,7 +9009,7 @@
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B224">
         <v>0</v>
@@ -9013,7 +9017,7 @@
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B225">
         <v>1</v>
@@ -9021,7 +9025,7 @@
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B226">
         <v>1</v>
@@ -9029,7 +9033,7 @@
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B227">
         <v>0</v>
@@ -9037,7 +9041,7 @@
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B228">
         <v>0</v>
@@ -9045,7 +9049,7 @@
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B229">
         <v>0</v>
@@ -9053,7 +9057,7 @@
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B230">
         <v>0</v>
@@ -9061,7 +9065,7 @@
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B231">
         <v>0</v>
@@ -9069,7 +9073,7 @@
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B232">
         <v>2</v>
@@ -9077,7 +9081,7 @@
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B233">
         <v>0</v>
@@ -9085,7 +9089,7 @@
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B234">
         <v>0</v>
@@ -9093,7 +9097,7 @@
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B235">
         <v>0</v>
@@ -9101,7 +9105,7 @@
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B236">
         <v>1</v>
@@ -9109,7 +9113,7 @@
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B237">
         <v>0</v>
@@ -9117,7 +9121,7 @@
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B238">
         <v>1</v>
@@ -9125,7 +9129,7 @@
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B239">
         <v>0</v>
@@ -9133,7 +9137,7 @@
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B240">
         <v>0</v>
@@ -9141,7 +9145,7 @@
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B241">
         <v>1</v>
@@ -9149,7 +9153,7 @@
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B242">
         <v>2</v>
@@ -9157,7 +9161,7 @@
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="B243">
         <v>2</v>
@@ -9165,7 +9169,7 @@
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B244">
         <v>0</v>
@@ -9173,7 +9177,7 @@
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="B245">
         <v>2</v>
@@ -9181,7 +9185,7 @@
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B246">
         <v>0</v>
@@ -9189,7 +9193,7 @@
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="B247">
         <v>0</v>
@@ -9197,7 +9201,7 @@
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B248">
         <v>1</v>
@@ -9205,7 +9209,7 @@
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="B249">
         <v>0</v>
@@ -9213,7 +9217,7 @@
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="B250">
         <v>2</v>
@@ -9221,7 +9225,7 @@
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B251">
         <v>2</v>
@@ -9229,7 +9233,7 @@
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="B252">
         <v>2</v>
@@ -9237,5 +9241,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>